<commit_message>
update tache du jour Gantt
</commit_message>
<xml_diff>
--- a/Docs/diagramme de Gantt.xlsx
+++ b/Docs/diagramme de Gantt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Documents\SAE 203\pong\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\iutbg-smbetu.univ-lyon1.fr\homes\Documents\SAE 203\pong\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC3F922-90C8-40AC-A700-F51D890A781C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1207F2-3D76-4880-B4F6-D5AA20C3B03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A73F89E-F015-4D54-8199-E6CADEF4336D}"/>
   </bookViews>
@@ -565,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -575,15 +575,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -629,6 +625,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799E04C-509C-4F2B-9BF9-E3486FBFB459}">
-  <dimension ref="A1:U40"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,31 +980,31 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="45" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1007,118 +1012,118 @@
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="52"/>
+      <c r="I5" s="48"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="52"/>
+      <c r="I6" s="48"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="52"/>
+      <c r="I7" s="48"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="53"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="52"/>
+      <c r="I8" s="48"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="52"/>
+      <c r="I9" s="48"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="56"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="52"/>
+      <c r="I10" s="48"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="52"/>
+      <c r="I11" s="48"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="52"/>
+      <c r="I12" s="48"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="59"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="55"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
@@ -1130,7 +1135,7 @@
       <c r="E17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="47" t="s">
+      <c r="F17" s="43" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1149,65 +1154,65 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="J25" s="34"/>
+      <c r="J25" s="30"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J26" s="34"/>
+      <c r="J26" s="30"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="G27" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="H27" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="31" t="s">
+      <c r="I27" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J27" s="34"/>
+      <c r="J27" s="30"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="13">
         <v>1</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="34"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
@@ -1216,23 +1221,23 @@
       <c r="B29" s="8">
         <v>1</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="34"/>
-      <c r="O29" s="34"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="34"/>
-      <c r="R29" s="34"/>
-      <c r="S29" s="34"/>
-      <c r="T29" s="34"/>
-      <c r="U29" s="34"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -1241,146 +1246,150 @@
       <c r="B30" s="8">
         <v>1</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="34"/>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
-      <c r="S30" s="34"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="34"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="30"/>
+      <c r="U30" s="30"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="18">
         <v>1</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="34"/>
-      <c r="O31" s="34"/>
-      <c r="P31" s="34"/>
-      <c r="Q31" s="34"/>
-      <c r="R31" s="34"/>
-      <c r="S31" s="34"/>
-      <c r="T31" s="34"/>
-      <c r="U31" s="34"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="30"/>
+      <c r="U31" s="30"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="36">
-        <v>0.2</v>
-      </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="34"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="34"/>
-      <c r="S32" s="34"/>
-      <c r="T32" s="34"/>
-      <c r="U32" s="34"/>
+      <c r="B32" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="30"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="34">
         <v>1</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27" t="s">
+      <c r="C33" s="22"/>
+      <c r="D33" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="34"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="34"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="34"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="39" t="s">
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="30"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="40">
+      <c r="B34" s="61">
         <v>1</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="34"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="30"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="16">
-        <v>0</v>
-      </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="19"/>
+      <c r="B35" s="65">
+        <v>0.7</v>
+      </c>
+      <c r="C35" s="66"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="40"/>
     </row>
     <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="14"/>
+      <c r="B36" s="36">
+        <v>0.4</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="42"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="67"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="67"/>
       <c r="C40" s="1" t="s">
         <v>16</v>
       </c>
@@ -1390,7 +1399,7 @@
       <c r="E40" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="47" t="s">
+      <c r="F40" s="43" t="s">
         <v>11</v>
       </c>
       <c r="G40" s="1" t="s">
@@ -1399,6 +1408,18 @@
       <c r="H40" s="1" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="67"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="67"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="67"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>